<commit_message>
internship and nav modified
admin side and client side internship done
</commit_message>
<xml_diff>
--- a/doc/placementdata.xlsx
+++ b/doc/placementdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Placement data</t>
   </si>
@@ -57,15 +57,6 @@
   </si>
   <si>
     <t>hchsh@hs.zz</t>
-  </si>
-  <si>
-    <t>nihip</t>
-  </si>
-  <si>
-    <t>LSD</t>
-  </si>
-  <si>
-    <t>111111111111</t>
   </si>
 </sst>
 </file>
@@ -404,7 +395,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -417,7 +408,7 @@
     <col min="3" max="3" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="15.281982" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="15.281982" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="15.281982" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="13.996582" bestFit="true" customWidth="true" style="0"/>
   </cols>
@@ -476,32 +467,6 @@
         <v>1122334455</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>1234</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>1122334455</v>
-      </c>
-      <c r="H5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>